<commit_message>
diccionario de variables para contactos
</commit_message>
<xml_diff>
--- a/interoperabilidad/diccionario-de-variables.xlsx
+++ b/interoperabilidad/diccionario-de-variables.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliver/Documents/MSPAS/godata-guatemala/interoperabilidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D766E08F-3FAA-D343-86CD-36D9DB775D8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E193865-FBF9-EC45-868A-8AF192646024}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{5E1ECCF0-DF51-B049-8E26-CB677146498A}"/>
+    <workbookView xWindow="900" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="3" xr2:uid="{5E1ECCF0-DF51-B049-8E26-CB677146498A}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos" sheetId="1" r:id="rId1"/>
-    <sheet name="Posibles valores" sheetId="2" r:id="rId2"/>
+    <sheet name="Contactos" sheetId="3" r:id="rId2"/>
+    <sheet name="Relacionar contacto a caso" sheetId="4" r:id="rId3"/>
+    <sheet name="Seguimiento de contactos" sheetId="5" r:id="rId4"/>
+    <sheet name="Posibles valores" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="477">
   <si>
     <t>Variables del modelo de Nuevo Caso</t>
   </si>
@@ -1178,6 +1181,294 @@
   </si>
   <si>
     <t>Valores</t>
+  </si>
+  <si>
+    <t>riskLevel</t>
+  </si>
+  <si>
+    <t>Nombres de los contacto</t>
+  </si>
+  <si>
+    <t>Apellidos del contacto</t>
+  </si>
+  <si>
+    <t>Género del contacto</t>
+  </si>
+  <si>
+    <t>Información de la edad del contacto</t>
+  </si>
+  <si>
+    <t>Edad en años del contacto</t>
+  </si>
+  <si>
+    <t>Nivel de riesgo que tiene el contacto de volverse un caso</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_RISK_LEVEL</t>
+  </si>
+  <si>
+    <t>typeId</t>
+  </si>
+  <si>
+    <t>Tipo de residencia</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_ADDRESS_TYPE_USUAL_PLACE_OF_RESIDENCE</t>
+  </si>
+  <si>
+    <t>Esta variable se manda con ese valor por default</t>
+  </si>
+  <si>
+    <t>dateOfLastContact</t>
+  </si>
+  <si>
+    <t>Fecha en la que el contacto tuvo el ultimo contacto con el caso.</t>
+  </si>
+  <si>
+    <t>En caso no se tenga esta información utilizar la fecha de notifiación.</t>
+  </si>
+  <si>
+    <t>followUp</t>
+  </si>
+  <si>
+    <t>Información de los seguimientos del contacto</t>
+  </si>
+  <si>
+    <t>originalStartDate</t>
+  </si>
+  <si>
+    <t>Fecha de inicio de seguimiento</t>
+  </si>
+  <si>
+    <t>Usualmente es el dia siguiente al de notificación</t>
+  </si>
+  <si>
+    <t>startDate</t>
+  </si>
+  <si>
+    <t>Fecha original de inicio de seguimiento</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_FINAL_FOLLOW_UP_STATUS_TYPE</t>
+  </si>
+  <si>
+    <t>Estado de seguimiento del contacto</t>
+  </si>
+  <si>
+    <t>Al entrar al sistema debe ingresar como bajo seguimiento</t>
+  </si>
+  <si>
+    <t>Variables del modelo relacionar un contacto a un caso</t>
+  </si>
+  <si>
+    <t>persons</t>
+  </si>
+  <si>
+    <t>Aca va el contacto que se desea relacionar al caso</t>
+  </si>
+  <si>
+    <t>El ID de Go.Data del contacto que se desea relacionar al caso</t>
+  </si>
+  <si>
+    <t>contactDate</t>
+  </si>
+  <si>
+    <t>Fecha en la que el ultimo contacto con el caso</t>
+  </si>
+  <si>
+    <t>Si no se tiene la info poner la fecha de notificación.</t>
+  </si>
+  <si>
+    <t>contactDateEstimated</t>
+  </si>
+  <si>
+    <t>Si la fecha de contacto es estimada</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Se utiliza false por default</t>
+  </si>
+  <si>
+    <t>certaintyLevelId</t>
+  </si>
+  <si>
+    <t>Nivel de riesgo del contacto a con el caso</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_CERTAINTY_LEVEL</t>
+  </si>
+  <si>
+    <t>people</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Variable que se manda por default</t>
+  </si>
+  <si>
+    <t>dateOfFirstContact</t>
+  </si>
+  <si>
+    <t>Fecha en la que el contacto tuvo el primer contacto con el caso</t>
+  </si>
+  <si>
+    <t>Si no se tiene la información poner la fecha de último contacto.</t>
+  </si>
+  <si>
+    <t>Variables del modelo de seguimientos de contactos</t>
+  </si>
+  <si>
+    <t>Fecha del seguimiento</t>
+  </si>
+  <si>
+    <t>targeted</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Esta es una variable que se manda por default.</t>
+  </si>
+  <si>
+    <t>statusId</t>
+  </si>
+  <si>
+    <t>El resultado del seguimiento</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_DAILY_FOLLOW_UP_STATUS_TYPE</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_RISK_LEVEL_1_LOW</t>
+  </si>
+  <si>
+    <t>1 - Bajo</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_RISK_LEVEL_2_MEDIUM</t>
+  </si>
+  <si>
+    <t>2 - Medio</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_RISK_LEVEL_3_HIGH</t>
+  </si>
+  <si>
+    <t>3 - Alta</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_FINAL_FOLLOW_UP_STATUS_TYPE_DIED</t>
+  </si>
+  <si>
+    <t>Murió</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_FINAL_FOLLOW_UP_STATUS_TYPE_FOLLOW_UP_COMPLETED</t>
+  </si>
+  <si>
+    <t>Seguimiento Completo</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_FINAL_FOLLOW_UP_STATUS_TYPE_LOST_TO_FOLLOW_UP</t>
+  </si>
+  <si>
+    <t>Perdido durante el seguimiento</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_FINAL_FOLLOW_UP_STATUS_TYPE_NEVER_ILL_NOT_A_CASE</t>
+  </si>
+  <si>
+    <t>Nunca Enfermo / No Es Un Caso</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_FINAL_FOLLOW_UP_STATUS_TYPE_SE_CONVIERTO_EN_UN_CASO</t>
+  </si>
+  <si>
+    <t>Se convirtió en caso</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_FINAL_FOLLOW_UP_STATUS_TYPE_SE_CONVIERTO_EN_UN_CASO_DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se convierto en un caso </t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_FINAL_FOLLOW_UP_STATUS_TYPE_UNDER_FOLLOW_UP</t>
+  </si>
+  <si>
+    <t>Bajo Seguimiento</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_CERTAINTY_LEVEL_1_LOW</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_CERTAINTY_LEVEL_2_MEDIUM</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_CERTAINTY_LEVEL_3_HIGH</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_CERTAINTY_LEVEL_CONTACTO_CERCANO_MENOS_DE_1_5_MTS</t>
+  </si>
+  <si>
+    <t>Contacto cercano (menos de 1.5 mts)</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_CERTAINTY_LEVEL_CONTACTO_DIRECTO_PERMANECE_EN_EL_MISMO_ENTORNO_CERCANO</t>
+  </si>
+  <si>
+    <t>Contacto directo (permanece en el mismo entorno cercano)</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_CERTAINTY_LEVEL_CONTACTO_INDIRECTO_VIAJAR_JUNTOS_1_METRO</t>
+  </si>
+  <si>
+    <t>Contacto indirecto - Viajar juntos (1 metro)</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_CERTAINTY_LEVEL_MIGRANTE</t>
+  </si>
+  <si>
+    <t>Migrante</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CATEGORY_CERTAINTY_LEVEL_VIVE_EN_EL_MISMO_LUGAR</t>
+  </si>
+  <si>
+    <t>Vive en el mismo lugar</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_DAILY_FOLLOW_UP_STATUS_TYPE_MISSED</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_DAILY_FOLLOW_UP_STATUS_TYPE_NOT_ATTEMPTED</t>
+  </si>
+  <si>
+    <t>No intentado</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_DAILY_FOLLOW_UP_STATUS_TYPE_NOT_PERFORMED</t>
+  </si>
+  <si>
+    <t>No Realizado</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_DAILY_FOLLOW_UP_STATUS_TYPE_SEEN_NOT_OK</t>
+  </si>
+  <si>
+    <t>Visto, no bien (con síntomas)</t>
+  </si>
+  <si>
+    <t>LNG_REFERENCE_DATA_CONTACT_DAILY_FOLLOW_UP_STATUS_TYPE_SEEN_OK</t>
+  </si>
+  <si>
+    <t>Visto, esta bien (sin síntomas)</t>
   </si>
 </sst>
 </file>
@@ -1260,9 +1551,6 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1272,12 +1560,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1285,7 +1576,124 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1360,6 +1768,9 @@
       </font>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1376,9 +1787,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1412,20 +1820,62 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8325F06-CC1B-734D-A84C-8224D788B209}" name="Tabla1" displayName="Tabla1" ref="A3:D124" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A3:D124" xr:uid="{4392FBBD-5A2D-FF41-AB39-7B4248AE40AE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8325F06-CC1B-734D-A84C-8224D788B209}" name="Tabla1" displayName="Tabla1" ref="A3:D125" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A3:D125" xr:uid="{4392FBBD-5A2D-FF41-AB39-7B4248AE40AE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D24CB07B-8001-8E40-8485-BCC6F5CF3F83}" name="Variable" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{BFCE3BF8-25DC-A749-9497-86DBC4AFEE2E}" name="Definición" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{D24CB07B-8001-8E40-8485-BCC6F5CF3F83}" name="Variable" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{BFCE3BF8-25DC-A749-9497-86DBC4AFEE2E}" name="Definición" dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{081E1926-0DFD-FE49-91BD-74419E63228A}" name="Valores"/>
     <tableColumn id="4" xr3:uid="{4C1E63C1-9DD3-9E4A-8AF1-3E957A694226}" name="Comentarios"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4FC7F15B-B10C-5B43-8445-B0450CF6CF21}" name="Tabla10" displayName="Tabla10" ref="G2:H14" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E76BBBAE-B22C-6F48-AC5E-52B01802879F}" name="Tabla7" displayName="Tabla7" ref="D2:E7" totalsRowShown="0">
+  <autoFilter ref="D2:E7" xr:uid="{673DE8BC-D535-0947-845E-CABBF228468E}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{41DEBB25-B84B-C941-A7E4-0D56C97BE79B}" name="key"/>
+    <tableColumn id="2" xr3:uid="{D4A2857F-6ADC-D547-AE3D-1760ACD0CA34}" name="value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7DA3AC0A-CA5F-CA4D-9DD6-D50537E0902A}" name="Tabla8" displayName="Tabla8" ref="D11:E16" totalsRowShown="0">
+  <autoFilter ref="D11:E16" xr:uid="{6EBB97E3-F3A2-F241-835C-1FFB5F9D1D2D}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{31023353-454F-E64A-958D-984E526419BC}" name="key"/>
+    <tableColumn id="2" xr3:uid="{68FF7C78-B557-5D4C-9401-42258C5C2962}" name="value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2C6EFC31-B808-3D4D-81FF-77CEF2F3E409}" name="Tabla9" displayName="Tabla9" ref="D20:E22" totalsRowShown="0">
+  <autoFilter ref="D20:E22" xr:uid="{CE354E05-8BDC-1046-BDB7-FF4665307348}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{2D2D3C3F-7814-B143-89DE-3F117248750F}" name="key"/>
+    <tableColumn id="2" xr3:uid="{077834C9-BDD4-EE4C-B5E6-6459432A8C50}" name="value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4FC7F15B-B10C-5B43-8445-B0450CF6CF21}" name="Tabla10" displayName="Tabla10" ref="G2:H14" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="G2:H14" xr:uid="{5A895AB7-14EA-F449-B2D3-216BE333B03E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1438,7 +1888,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7E169EFF-15B3-8549-BF72-9535C834FE36}" name="Tabla11" displayName="Tabla11" ref="G17:H31" totalsRowShown="0">
   <autoFilter ref="G17:H31" xr:uid="{F8384FAD-11E5-9F41-848D-888D35574EBF}"/>
   <tableColumns count="2">
@@ -1449,7 +1899,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{1E2A75A4-2520-7F4E-BE97-ADF3DBC5FBE2}" name="Tabla12" displayName="Tabla12" ref="J2:K4" totalsRowShown="0">
   <autoFilter ref="J2:K4" xr:uid="{3B01CEE0-4FFF-D746-B8F2-B0E4D359BA20}"/>
   <tableColumns count="2">
@@ -1460,7 +1910,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{4CDB0AB9-3B6B-FB4D-A86B-CD3D23B5807A}" name="Tabla13" displayName="Tabla13" ref="J8:K12" totalsRowShown="0">
   <autoFilter ref="J8:K12" xr:uid="{A5D4C6AA-992B-CA45-83C2-98725F92A8CB}"/>
   <tableColumns count="2">
@@ -1471,7 +1921,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{76DC0193-E60F-C64B-9749-44044A259DB2}" name="Tabla14" displayName="Tabla14" ref="J16:K21" totalsRowShown="0">
   <autoFilter ref="J16:K21" xr:uid="{134A0818-4366-004C-9A76-379002461BB1}"/>
   <tableColumns count="2">
@@ -1482,7 +1932,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{59ED3080-AF8D-6541-8B32-8F06B2E6BCDD}" name="Tabla15" displayName="Tabla15" ref="M2:N8" totalsRowShown="0">
   <autoFilter ref="M2:N8" xr:uid="{90358D85-171F-D340-9685-99AA1509CB4C}"/>
   <tableColumns count="2">
@@ -1493,7 +1943,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{94317AED-B346-C744-9C2E-B49259B8C0A1}" name="Tabla16" displayName="Tabla16" ref="M11:N13" totalsRowShown="0">
   <autoFilter ref="M11:N13" xr:uid="{FC4F62F9-F608-354A-BFE3-2464513A2C47}"/>
   <tableColumns count="2">
@@ -1505,6 +1955,89 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{3588DEEC-E7BF-9446-B6CB-06BE52D922A5}" name="Tabla19" displayName="Tabla19" ref="A3:D23" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A3:D23" xr:uid="{B8BBF063-55EF-9348-913C-72EE1CFD6847}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FEF949F5-9F98-6345-8EE2-7006FA9E1AA1}" name="Variable"/>
+    <tableColumn id="2" xr3:uid="{1ED81021-2503-E641-B1D6-1A5DCF75CCA4}" name="Definición" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{B050EFA3-AF9C-5D4F-B827-F53AE6BB030E}" name="Valores"/>
+    <tableColumn id="4" xr3:uid="{AFFA3E39-19D8-2F45-8A25-64BCBA0CA120}" name="Comentarios" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{F14328BA-D33D-FC4D-99B8-375CEB1EBECF}" name="Tabla23" displayName="Tabla23" ref="P2:Q5" totalsRowShown="0">
+  <autoFilter ref="P2:Q5" xr:uid="{72BC0794-11D7-2144-A21E-0F91E9134A84}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{E54B2840-9A85-2049-98D1-D60605E453A5}" name="key"/>
+    <tableColumn id="2" xr3:uid="{14AD0CFD-73C3-5644-A986-6DE9D89F1390}" name="value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{BCBA47BC-E2F7-1145-B8A4-520395253C6D}" name="Tabla24" displayName="Tabla24" ref="P8:Q14" totalsRowShown="0">
+  <autoFilter ref="P8:Q14" xr:uid="{C1595F33-1755-9F4D-AB8A-1FE3912D92BD}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{0F425713-005A-B244-B3F2-701ACB8C44AB}" name="LNG_REFERENCE_DATA_CONTACT_FINAL_FOLLOW_UP_STATUS_TYPE_DIED"/>
+    <tableColumn id="2" xr3:uid="{8592A4FD-25A8-3247-B628-AC1DA5A5D2F6}" name="Murió"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{4915EAD9-0B3C-C245-AABF-ED97FC432D6D}" name="Tabla25" displayName="Tabla25" ref="P18:Q25" totalsRowShown="0">
+  <autoFilter ref="P18:Q25" xr:uid="{5E9A7224-EE64-7A44-8F73-C9B07676331C}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{52D85290-B6F3-C44A-AC5E-16042FC29C93}" name="LNG_REFERENCE_DATA_CATEGORY_CERTAINTY_LEVEL_1_LOW"/>
+    <tableColumn id="2" xr3:uid="{103ACE71-E3B3-7B4B-ABC6-3C18DA55A64F}" name="1 - Bajo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{9F41C477-007F-A146-9D5C-A5BDDE7F302D}" name="Tabla26" displayName="Tabla26" ref="S2:T6" totalsRowShown="0">
+  <autoFilter ref="S2:T6" xr:uid="{6DFF0F9C-D2FC-354A-B732-DE306F7D4416}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{DC85A796-E26C-A848-A60D-1091EAE1ECC3}" name="LNG_REFERENCE_DATA_CONTACT_DAILY_FOLLOW_UP_STATUS_TYPE_MISSED"/>
+    <tableColumn id="2" xr3:uid="{8E4C04BD-F109-5443-877A-39A34E46E5DA}" name="Perdido"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{697A7F60-BF99-DA45-ABCA-0FF98BFCA0A3}" name="Tabla21" displayName="Tabla21" ref="A3:D10" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A3:D10" xr:uid="{D19012DF-03D4-D547-AE22-4C57CB0A8687}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{7249162F-9EEF-714C-8ACF-DC9D7912F666}" name="Variable"/>
+    <tableColumn id="2" xr3:uid="{9C37ABA9-D436-6D49-9433-9D6CAA5E9298}" name="Definición" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{BB1CA97B-FF77-AE47-A621-6740FD8BCFBA}" name="Valores"/>
+    <tableColumn id="4" xr3:uid="{68C8A4C4-F4B4-EF41-ACB4-522C0082D9CA}" name="Comentarios" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{6A3E38CA-857E-724A-BAC9-43E4BE3B5777}" name="Tabla2123" displayName="Tabla2123" ref="A3:D6" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A3:D6" xr:uid="{5E38CC3C-9FA6-7342-AF3F-4F8A30942A9C}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0F5570D8-3507-3A4F-AFBF-C24F964B4B91}" name="Variable"/>
+    <tableColumn id="2" xr3:uid="{FFEC3E5F-5773-0C45-AC27-CD659E536223}" name="Definición" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{FC444456-4BC9-B946-AD9F-ABE259EFD4A0}" name="Valores"/>
+    <tableColumn id="4" xr3:uid="{E47EB35F-22C0-A044-9A51-7A86C932FE38}" name="Comentarios" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{769DED12-C8C7-3144-B0A9-74669E7C473D}" name="Tabla2" displayName="Tabla2" ref="A2:B4" totalsRowShown="0">
   <autoFilter ref="A2:B4" xr:uid="{E0117D06-AA75-7B49-A024-7ED0ADF12DBD}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -1518,7 +2051,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{26FDE5F7-70D3-C140-92B2-011A5B4CE412}" name="Tabla3" displayName="Tabla3" ref="M17:N24" totalsRowShown="0">
   <autoFilter ref="M17:N24" xr:uid="{E5C71A26-5098-E14A-8421-F38FD6C4137A}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -1532,21 +2065,21 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7B2DCCD7-105C-614C-AAC1-CB1597961238}" name="Tabla4" displayName="Tabla4" ref="A8:B11" totalsRowShown="0" dataDxfId="1">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7B2DCCD7-105C-614C-AAC1-CB1597961238}" name="Tabla4" displayName="Tabla4" ref="A8:B11" totalsRowShown="0" dataDxfId="12">
   <autoFilter ref="A8:B11" xr:uid="{1BB55BB2-1442-4440-A34C-5555D4DA6E98}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0AE98AA4-EC5A-A141-BAE8-A9B9E7ACB5B2}" name="key" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{2A97BAAB-686F-F44F-A313-694513AB7647}" name="value" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{0AE98AA4-EC5A-A141-BAE8-A9B9E7ACB5B2}" name="key" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{2A97BAAB-686F-F44F-A313-694513AB7647}" name="value" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9EC5DC79-94B1-8441-838F-0E5AFE43D6FB}" name="Tabla5" displayName="Tabla5" ref="A15:B19" totalsRowShown="0">
   <autoFilter ref="A15:B19" xr:uid="{6A8A027B-9939-6945-AF1B-ED2FB10A5060}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -1560,54 +2093,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C30664FD-90CE-E84F-A7CE-2582E1EE5D95}" name="Tabla6" displayName="Tabla6" ref="A23:B32" totalsRowShown="0">
   <autoFilter ref="A23:B32" xr:uid="{3A97FB9D-8071-544D-A1B4-CE498EFA1203}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{6A84FA28-52A0-0A4D-B93E-4EEEF2FDA243}" name="key"/>
     <tableColumn id="2" xr3:uid="{53D30119-CCD6-564C-88A0-648EE72B69D8}" name="value"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E76BBBAE-B22C-6F48-AC5E-52B01802879F}" name="Tabla7" displayName="Tabla7" ref="D2:E7" totalsRowShown="0">
-  <autoFilter ref="D2:E7" xr:uid="{673DE8BC-D535-0947-845E-CABBF228468E}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{41DEBB25-B84B-C941-A7E4-0D56C97BE79B}" name="key"/>
-    <tableColumn id="2" xr3:uid="{D4A2857F-6ADC-D547-AE3D-1760ACD0CA34}" name="value"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7DA3AC0A-CA5F-CA4D-9DD6-D50537E0902A}" name="Tabla8" displayName="Tabla8" ref="D11:E16" totalsRowShown="0">
-  <autoFilter ref="D11:E16" xr:uid="{6EBB97E3-F3A2-F241-835C-1FFB5F9D1D2D}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{31023353-454F-E64A-958D-984E526419BC}" name="key"/>
-    <tableColumn id="2" xr3:uid="{68FF7C78-B557-5D4C-9401-42258C5C2962}" name="value"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2C6EFC31-B808-3D4D-81FF-77CEF2F3E409}" name="Tabla9" displayName="Tabla9" ref="D20:E22" totalsRowShown="0">
-  <autoFilter ref="D20:E22" xr:uid="{CE354E05-8BDC-1046-BDB7-FF4665307348}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2D2D3C3F-7814-B143-89DE-3F117248750F}" name="key"/>
-    <tableColumn id="2" xr3:uid="{077834C9-BDD4-EE4C-B5E6-6459432A8C50}" name="value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1910,10 +2401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC65D3B-CDCB-8348-94E6-69E3CEC3E469}">
-  <dimension ref="A2:D124"/>
+  <dimension ref="A2:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView zoomScale="98" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1925,24 +2416,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1950,10 +2441,10 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1961,10 +2452,10 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1972,13 +2463,13 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1986,13 +2477,13 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2000,7 +2491,7 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2008,7 +2499,7 @@
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2016,10 +2507,10 @@
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2027,7 +2518,7 @@
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2035,13 +2526,13 @@
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2049,10 +2540,10 @@
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2060,13 +2551,13 @@
       <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2074,1092 +2565,1106 @@
       <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>37</v>
+    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D16" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="C28" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C29" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="C32" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C33" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B34" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C35" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B36" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C37" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B38" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B39" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="C39" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B40" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B41" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C41" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B42" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>98</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B43" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>185</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C44" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="C45" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="C45" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="C46" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="C46" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+      <c r="C47" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C47" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+      <c r="C48" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="C48" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+      <c r="C49" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="C49" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+      <c r="C50" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+      <c r="C51" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C51" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+      <c r="C52" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="C52" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
+      <c r="C53" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="C53" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+      <c r="C54" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="C54" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
+      <c r="C55" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
+      <c r="C56" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="C56" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
+      <c r="C57" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="C57" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+      <c r="C58" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C58" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
+      <c r="C59" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="C59" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+      <c r="C60" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="C60" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
+      <c r="C61" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="C61" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="C62" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="C62" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+      <c r="C63" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="C63" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
+      <c r="C64" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="C64" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+      <c r="C65" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B66" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B67" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B68" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B69" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B70" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+    <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B71" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+    <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B72" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B73" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+    <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B74" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+    <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
+    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B76" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+    <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B77" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
+    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B78" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
+    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B79" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
+    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B80" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
+    <row r="81" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B81" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
+    <row r="82" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B82" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
+    <row r="83" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B83" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
+    <row r="84" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B84" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="4" t="s">
+    <row r="85" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B85" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
+    <row r="86" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B86" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
+    <row r="87" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B87" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
+    <row r="88" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B88" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="s">
+    <row r="89" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B89" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="s">
+    <row r="90" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="s">
+    <row r="91" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B91" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="s">
+    <row r="92" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B92" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="s">
+    <row r="93" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B93" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="4" t="s">
+    <row r="94" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B94" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="4" t="s">
+    <row r="95" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B95" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="s">
+    <row r="96" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B96" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="4" t="s">
+    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B97" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="4" t="s">
+    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B98" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" s="4" t="s">
+    <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B99" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="4" t="s">
+    <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B100" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="4" t="s">
+    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B101" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A101" s="4" t="s">
+    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B102" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="4" t="s">
+    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B103" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="4" t="s">
+    <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B104" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="4" t="s">
+    <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B105" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" s="4" t="s">
+    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B106" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="C105" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="4" t="s">
+      <c r="C106" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B107" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="C106" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="4" t="s">
+      <c r="C107" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B108" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="C107" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="4" t="s">
+      <c r="C108" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B109" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="C108" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="4" t="s">
+      <c r="C109" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B110" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="C109" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
+      <c r="C110" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B111" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="C110" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A111" s="4" t="s">
+      <c r="C111" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B112" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="C111" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A112" s="4" t="s">
+      <c r="C112" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B113" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="C112" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A113" s="4" t="s">
+      <c r="C113" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B114" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="C113" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A114" s="4" t="s">
+      <c r="C114" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B115" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="C114" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A115" s="4" t="s">
+      <c r="C115" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B116" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="C115" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A116" s="4" t="s">
+      <c r="C116" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B117" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="C116" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A117" s="4" t="s">
+      <c r="C117" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B118" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="C117" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A118" s="4" t="s">
+      <c r="C118" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B119" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="C118" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A119" s="4" t="s">
+      <c r="C119" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B120" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="C119" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="4" t="s">
+      <c r="C120" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B121" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="C120" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="4" t="s">
+      <c r="C121" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B122" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="C121" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" s="4" t="s">
+      <c r="C122" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B123" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C122" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A123" s="4" t="s">
+      <c r="C123" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B124" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="C123" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A124" s="4" t="s">
+      <c r="C124" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A125" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B125" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="C124" s="11" t="s">
+      <c r="C125" s="9" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3168,23 +3673,23 @@
     <mergeCell ref="A2:D2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C7" location="'Respuestas cerradas'!A1" display="LNG_REFERENCE_DATA_CATEGORY_GENDER" xr:uid="{A4E577B3-F0EA-3946-9A4A-BB2639B0C7CA}"/>
-    <hyperlink ref="C12" location="'Respuestas cerradas'!A7" display="LNG_REFERENCE_DATA_CATEGORY_OUTCOME" xr:uid="{3907F9E7-D1EE-F74E-B05B-E825CAAAF9F1}"/>
-    <hyperlink ref="C14" location="'Respuestas cerradas'!A14" display="LNG_REFERENCE_DATA_CATEGORY_CASE_CLASSIFICATION" xr:uid="{B556AFD1-4738-744D-ACA1-F36A5E9F22CE}"/>
-    <hyperlink ref="C21" location="'Respuestas cerradas'!A22" display="LNG_REFERENCE_DATA_CATEGORY_PREGNANCY_STATUS" xr:uid="{004A2061-B729-4E4C-9018-16C9F8C51CF1}"/>
-    <hyperlink ref="C27" location="'Respuestas cerradas'!D1" display="value" xr:uid="{357F2258-F3FF-FD4E-8E7F-DB77F4F854C0}"/>
-    <hyperlink ref="C28" location="'Respuestas cerradas'!D10" display="value" xr:uid="{B0D29223-D35B-264B-93BC-EA5935355F1A}"/>
-    <hyperlink ref="C31" location="'Respuestas cerradas'!D19" display="value" xr:uid="{A82223C6-B93E-C44C-9EB1-D3C1004F8C4A}"/>
-    <hyperlink ref="C32" location="'Respuestas cerradas'!G1" display="value" xr:uid="{79199AE9-6A7C-1F47-AFAC-C8CF4EE789C6}"/>
-    <hyperlink ref="C34" location="'Respuestas cerradas'!G16" display="value" xr:uid="{3023810B-154A-104A-8D03-FFF47701D425}"/>
-    <hyperlink ref="C36" location="'Respuestas cerradas'!J1" display="value" xr:uid="{349ED3B1-1148-3944-B9B5-8869EAEDA28B}"/>
-    <hyperlink ref="C38" location="'Respuestas cerradas'!J7" display="value" xr:uid="{9AC6C71A-4F48-3B4A-A31F-E48CD3765CBB}"/>
-    <hyperlink ref="C40" location="'Respuestas cerradas'!J15" display="value" xr:uid="{1EFCC6DF-8C0E-D44A-8265-BDA0A05D2BBA}"/>
-    <hyperlink ref="C44" location="'Respuestas cerradas'!M1" display="value" xr:uid="{78DBEA77-A3C3-1A4D-96E6-31609720E779}"/>
-    <hyperlink ref="C45" location="'Respuestas cerradas'!M10" display="value" xr:uid="{29CCC6FC-BB37-E44D-A8AC-C5A579CC8DC8}"/>
-    <hyperlink ref="C46:C64" location="'Respuestas cerradas'!M10" display="value" xr:uid="{C674B9CB-4E14-0447-89E3-3C4618EFB573}"/>
-    <hyperlink ref="C105" location="'Respuestas cerradas'!M16" display="value" xr:uid="{6B8DCF13-0056-C94D-92C7-03A91AFA7EE0}"/>
-    <hyperlink ref="C106:C124" location="'Respuestas cerradas'!M16" display="value" xr:uid="{81EF66AF-6A4D-D941-A3CA-3324CBF4548C}"/>
+    <hyperlink ref="C7" location="'Posibles valores'!A1" display="LNG_REFERENCE_DATA_CATEGORY_GENDER" xr:uid="{A4E577B3-F0EA-3946-9A4A-BB2639B0C7CA}"/>
+    <hyperlink ref="C12" location="'Posibles valores'!A7" display="LNG_REFERENCE_DATA_CATEGORY_OUTCOME" xr:uid="{3907F9E7-D1EE-F74E-B05B-E825CAAAF9F1}"/>
+    <hyperlink ref="C14" location="'Posibles valores'!A14" display="LNG_REFERENCE_DATA_CATEGORY_CASE_CLASSIFICATION" xr:uid="{B556AFD1-4738-744D-ACA1-F36A5E9F22CE}"/>
+    <hyperlink ref="C22" location="'Posibles valores'!A22" display="LNG_REFERENCE_DATA_CATEGORY_PREGNANCY_STATUS" xr:uid="{004A2061-B729-4E4C-9018-16C9F8C51CF1}"/>
+    <hyperlink ref="C28" location="'Posibles valores'!D1" display="value" xr:uid="{357F2258-F3FF-FD4E-8E7F-DB77F4F854C0}"/>
+    <hyperlink ref="C29" location="'Posibles valores'!D10" display="value" xr:uid="{B0D29223-D35B-264B-93BC-EA5935355F1A}"/>
+    <hyperlink ref="C32" location="'Posibles valores'!D19" display="value" xr:uid="{A82223C6-B93E-C44C-9EB1-D3C1004F8C4A}"/>
+    <hyperlink ref="C33" location="'Posibles valores'!G1" display="value" xr:uid="{79199AE9-6A7C-1F47-AFAC-C8CF4EE789C6}"/>
+    <hyperlink ref="C35" location="'Posibles valores'!G16" display="value" xr:uid="{3023810B-154A-104A-8D03-FFF47701D425}"/>
+    <hyperlink ref="C37" location="'Posibles valores'!J1" display="value" xr:uid="{349ED3B1-1148-3944-B9B5-8869EAEDA28B}"/>
+    <hyperlink ref="C39" location="'Posibles valores'!J7" display="value" xr:uid="{9AC6C71A-4F48-3B4A-A31F-E48CD3765CBB}"/>
+    <hyperlink ref="C41" location="'Posibles valores'!J15" display="value" xr:uid="{1EFCC6DF-8C0E-D44A-8265-BDA0A05D2BBA}"/>
+    <hyperlink ref="C45" location="'Posibles valores'!M1" display="value" xr:uid="{78DBEA77-A3C3-1A4D-96E6-31609720E779}"/>
+    <hyperlink ref="C46" location="'Posibles valores'!M10" display="value" xr:uid="{29CCC6FC-BB37-E44D-A8AC-C5A579CC8DC8}"/>
+    <hyperlink ref="C106" location="'Posibles valores'!M16" display="value" xr:uid="{6B8DCF13-0056-C94D-92C7-03A91AFA7EE0}"/>
+    <hyperlink ref="C107:C125" location="'Respuestas cerradas'!M16" display="value" xr:uid="{81EF66AF-6A4D-D941-A3CA-3324CBF4548C}"/>
+    <hyperlink ref="C47:C65" location="'Posibles valores'!M10" display="value" xr:uid="{D3A83D42-2EEF-5049-A00C-3FD43E39E7E7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3194,11 +3699,500 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72457994-CA38-F345-AD29-992CA998C780}">
+  <dimension ref="A2:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>381</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D12" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>396</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>398</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>401</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>403</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C6" location="'Posibles valores'!A1" display="LNG_REFERENCE_DATA_CATEGORY_GENDER" xr:uid="{BAC9F552-4C75-2F48-8193-260A749E8DC1}"/>
+    <hyperlink ref="C23" location="'Posibles valores'!A22" display="LNG_REFERENCE_DATA_CATEGORY_PREGNANCY_STATUS" xr:uid="{428993F9-A017-2547-AC3E-C9BA199D96E1}"/>
+    <hyperlink ref="C10" location="'Posibles valores'!P1" display="LNG_REFERENCE_DATA_CATEGORY_RISK_LEVEL" xr:uid="{D535379D-F12F-2844-88ED-8E76FC40AE47}"/>
+    <hyperlink ref="C22" location="'Posibles valores'!P7" display="LNG_REFERENCE_DATA_CONTACT_FINAL_FOLLOW_UP_STATUS_TYPE" xr:uid="{59A43E76-5549-E840-9077-6C723613A35A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFFE545-A25A-744D-8811-5DA0DAFBF868}">
+  <dimension ref="A2:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>411</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>414</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C7" t="s">
+        <v>416</v>
+      </c>
+      <c r="D7" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>418</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>421</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>424</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C8" location="'Posibles valores'!P17" display="LNG_REFERENCE_DATA_CATEGORY_CERTAINTY_LEVEL" xr:uid="{248BB8FB-74DA-6246-865A-DF29B27889C5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD56939-C7F4-7443-AA86-9379DE574403}">
+  <dimension ref="A2:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>429</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C5" t="s">
+        <v>430</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>432</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C6" location="'Posibles valores'!S1" display="LNG_REFERENCE_DATA_CONTACT_DAILY_FOLLOW_UP_STATUS_TYPE" xr:uid="{E51968B5-3B0A-A448-8867-C606BF369D3B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A82A722-9A82-3D4F-96C1-760BF6340711}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:K15"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3211,31 +4205,43 @@
     <col min="8" max="8" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="44.83203125" customWidth="1"/>
     <col min="14" max="14" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="111.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="51" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="77.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:20" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="G1" s="12" t="s">
+      <c r="E1" s="11"/>
+      <c r="G1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="J1" s="12" t="s">
+      <c r="H1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="M1" s="12" t="s">
+      <c r="K1" s="11"/>
+      <c r="M1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="N1" s="12"/>
-    </row>
-    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+      <c r="N1" s="11"/>
+      <c r="P1" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q1" s="11"/>
+      <c r="S1" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="T1" s="11"/>
+    </row>
+    <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3248,10 +4254,10 @@
       <c r="E2" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>67</v>
       </c>
       <c r="J2" t="s">
@@ -3266,8 +4272,20 @@
       <c r="N2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S2" t="s">
+        <v>468</v>
+      </c>
+      <c r="T2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>228</v>
       </c>
@@ -3283,7 +4301,7 @@
       <c r="G3" t="s">
         <v>98</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>293</v>
       </c>
       <c r="J3" t="s">
@@ -3298,8 +4316,20 @@
       <c r="N3" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P3" t="s">
+        <v>435</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>436</v>
+      </c>
+      <c r="S3" t="s">
+        <v>469</v>
+      </c>
+      <c r="T3" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>230</v>
       </c>
@@ -3330,8 +4360,20 @@
       <c r="N4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P4" t="s">
+        <v>437</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>438</v>
+      </c>
+      <c r="S4" t="s">
+        <v>471</v>
+      </c>
+      <c r="T4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>266</v>
       </c>
@@ -3350,8 +4392,20 @@
       <c r="N5" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P5" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>440</v>
+      </c>
+      <c r="S5" t="s">
+        <v>473</v>
+      </c>
+      <c r="T5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>267</v>
       </c>
@@ -3370,12 +4424,18 @@
       <c r="N6" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="S6" t="s">
+        <v>475</v>
+      </c>
+      <c r="T6" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="24" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="11"/>
       <c r="D7" t="s">
         <v>268</v>
       </c>
@@ -3388,18 +4448,22 @@
       <c r="H7" t="s">
         <v>289</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="12"/>
+      <c r="K7" s="11"/>
       <c r="M7" t="s">
         <v>268</v>
       </c>
       <c r="N7" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P7" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3424,12 +4488,18 @@
       <c r="N8" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="P8" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>233</v>
       </c>
       <c r="G9" t="s">
@@ -3444,18 +4514,24 @@
       <c r="K9" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="P9" t="s">
+        <v>443</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="24" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E10" s="11"/>
       <c r="G10" t="s">
         <v>282</v>
       </c>
@@ -3468,16 +4544,22 @@
       <c r="K10" t="s">
         <v>317</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="M10" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="N10" s="12"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="N10" s="11"/>
+      <c r="P10" t="s">
+        <v>445</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>237</v>
       </c>
       <c r="D11" t="s">
@@ -3504,8 +4586,14 @@
       <c r="N11" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P11" t="s">
+        <v>447</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>98</v>
       </c>
@@ -3530,8 +4618,14 @@
       <c r="N12" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P12" t="s">
+        <v>449</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>265</v>
       </c>
@@ -3550,12 +4644,18 @@
       <c r="N13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="P13" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="24" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="B14" s="12"/>
+      <c r="B14" s="11"/>
       <c r="D14" t="s">
         <v>266</v>
       </c>
@@ -3568,8 +4668,14 @@
       <c r="H14" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="P14" t="s">
+        <v>453</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -3582,12 +4688,12 @@
       <c r="E15" t="s">
         <v>277</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K15" s="12"/>
-    </row>
-    <row r="16" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="1:20" ht="24" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>239</v>
       </c>
@@ -3600,22 +4706,22 @@
       <c r="E16" t="s">
         <v>278</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="H16" s="12"/>
+      <c r="H16" s="11"/>
       <c r="J16" t="s">
         <v>9</v>
       </c>
       <c r="K16" t="s">
         <v>67</v>
       </c>
-      <c r="M16" s="12" t="s">
+      <c r="M16" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="N16" s="12"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>240</v>
       </c>
@@ -3640,8 +4746,12 @@
       <c r="N17" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P17" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="Q17" s="11"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>242</v>
       </c>
@@ -3666,18 +4776,24 @@
       <c r="N18" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="P18" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>241</v>
       </c>
       <c r="B19" t="s">
         <v>245</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="12"/>
+      <c r="E19" s="11"/>
       <c r="G19" t="s">
         <v>265</v>
       </c>
@@ -3696,8 +4812,14 @@
       <c r="N19" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P19" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>9</v>
       </c>
@@ -3722,8 +4844,14 @@
       <c r="N20" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P20" t="s">
+        <v>457</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>98</v>
       </c>
@@ -3748,12 +4876,18 @@
       <c r="N21" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
+      <c r="P21" t="s">
+        <v>458</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="12"/>
+      <c r="B22" s="11"/>
       <c r="D22" t="s">
         <v>265</v>
       </c>
@@ -3772,8 +4906,14 @@
       <c r="N22" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P22" t="s">
+        <v>460</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -3792,8 +4932,14 @@
       <c r="N23" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P23" t="s">
+        <v>462</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>247</v>
       </c>
@@ -3806,16 +4952,22 @@
       <c r="H24" t="s">
         <v>307</v>
       </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
       <c r="M24" t="s">
         <v>281</v>
       </c>
       <c r="N24" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P24" t="s">
+        <v>464</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>249</v>
       </c>
@@ -3828,8 +4980,14 @@
       <c r="H25" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P25" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>251</v>
       </c>
@@ -3843,7 +5001,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>253</v>
       </c>
@@ -3857,7 +5015,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>255</v>
       </c>
@@ -3871,7 +5029,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>257</v>
       </c>
@@ -3885,7 +5043,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>259</v>
       </c>
@@ -3899,7 +5057,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>261</v>
       </c>
@@ -3913,7 +5071,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>263</v>
       </c>
@@ -3922,14 +5080,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M16:N16"/>
+  <mergeCells count="20">
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A14:B14"/>
@@ -3939,9 +5094,16 @@
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M16:N16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="15">
+  <tableParts count="19">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -3957,6 +5119,10 @@
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
     <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>